<commit_message>
Adding xcos simultion; organizing control analysis better
</commit_message>
<xml_diff>
--- a/Control Analysis/DeltaF calcs.xlsx
+++ b/Control Analysis/DeltaF calcs.xlsx
@@ -462,127 +462,127 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="41"/>
                 <c:pt idx="0">
-                  <c:v>-30</c:v>
+                  <c:v>-20</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>-24.75</c:v>
+                  <c:v>-14.75</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>-19.5</c:v>
+                  <c:v>-9.5</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>-14.25</c:v>
+                  <c:v>-4.25</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>-9</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>-3.75</c:v>
+                  <c:v>6.25</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>1.5</c:v>
+                  <c:v>11.5</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>6.75</c:v>
+                  <c:v>16.75</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>12</c:v>
+                  <c:v>22</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>17.25</c:v>
+                  <c:v>27.25</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>22.5</c:v>
+                  <c:v>32.5</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>27.75</c:v>
+                  <c:v>37.75</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>33</c:v>
+                  <c:v>43</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>38.25</c:v>
+                  <c:v>48.25</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>43.5</c:v>
+                  <c:v>53.5</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>48.75</c:v>
+                  <c:v>58.75</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>54</c:v>
+                  <c:v>64</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>59.25</c:v>
+                  <c:v>69.25</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>64.5</c:v>
+                  <c:v>74.5</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>69.75</c:v>
+                  <c:v>79.75</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>75</c:v>
+                  <c:v>85</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>80.25</c:v>
+                  <c:v>90.25</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>85.5</c:v>
+                  <c:v>95.5</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>90.75</c:v>
+                  <c:v>100.75</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>96</c:v>
+                  <c:v>106</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>101.25</c:v>
+                  <c:v>111.25</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>106.5</c:v>
+                  <c:v>116.5</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>111.75</c:v>
+                  <c:v>121.75</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>117</c:v>
+                  <c:v>127</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>122.25</c:v>
+                  <c:v>132.25</c:v>
                 </c:pt>
                 <c:pt idx="30">
-                  <c:v>127.5</c:v>
+                  <c:v>137.5</c:v>
                 </c:pt>
                 <c:pt idx="31">
-                  <c:v>132.75</c:v>
+                  <c:v>142.75</c:v>
                 </c:pt>
                 <c:pt idx="32">
-                  <c:v>138</c:v>
+                  <c:v>148</c:v>
                 </c:pt>
                 <c:pt idx="33">
-                  <c:v>143.25</c:v>
+                  <c:v>153.25</c:v>
                 </c:pt>
                 <c:pt idx="34">
-                  <c:v>148.5</c:v>
+                  <c:v>158.5</c:v>
                 </c:pt>
                 <c:pt idx="35">
-                  <c:v>153.75</c:v>
+                  <c:v>163.75</c:v>
                 </c:pt>
                 <c:pt idx="36">
-                  <c:v>159</c:v>
+                  <c:v>169</c:v>
                 </c:pt>
                 <c:pt idx="37">
-                  <c:v>164.25</c:v>
+                  <c:v>174.25</c:v>
                 </c:pt>
                 <c:pt idx="38">
-                  <c:v>169.5</c:v>
+                  <c:v>179.5</c:v>
                 </c:pt>
                 <c:pt idx="39">
-                  <c:v>174.75</c:v>
+                  <c:v>184.75</c:v>
                 </c:pt>
                 <c:pt idx="40">
-                  <c:v>180</c:v>
+                  <c:v>190</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -597,124 +597,124 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1.1250000000000001E-2</c:v>
+                  <c:v>8.7500000000000008E-3</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>2.2500000000000003E-2</c:v>
+                  <c:v>1.7500000000000002E-2</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>3.3750000000000002E-2</c:v>
+                  <c:v>2.6250000000000002E-2</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>4.5000000000000005E-2</c:v>
+                  <c:v>3.5000000000000003E-2</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>5.6250000000000001E-2</c:v>
+                  <c:v>4.3750000000000004E-2</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>6.7500000000000004E-2</c:v>
+                  <c:v>5.2500000000000005E-2</c:v>
                 </c:pt>
                 <c:pt idx="7">
+                  <c:v>6.1250000000000006E-2</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>7.0000000000000007E-2</c:v>
+                </c:pt>
+                <c:pt idx="9">
                   <c:v>7.8750000000000001E-2</c:v>
                 </c:pt>
-                <c:pt idx="8">
-                  <c:v>9.0000000000000011E-2</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>0.10125000000000001</c:v>
-                </c:pt>
                 <c:pt idx="10">
-                  <c:v>0.1125</c:v>
+                  <c:v>8.7500000000000008E-2</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>0.12375000000000001</c:v>
+                  <c:v>9.6250000000000002E-2</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>0.13500000000000001</c:v>
+                  <c:v>0.10156122448979592</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>0.14625000000000002</c:v>
+                  <c:v>0.11180676020408163</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>0.15209375</c:v>
+                  <c:v>0.13161479591836733</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>0.1630859375</c:v>
+                  <c:v>0.16098533163265305</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>0.1835</c:v>
+                  <c:v>0.19991836734693877</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>0.21333593749999999</c:v>
+                  <c:v>0.24841390306122449</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>0.25259375000000001</c:v>
+                  <c:v>0.30647193877551016</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>0.30127343750000002</c:v>
+                  <c:v>0.37409247448979588</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>0.359375</c:v>
+                  <c:v>0.45127551020408163</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>0.42689843750000001</c:v>
+                  <c:v>0.5380210459183673</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>0.50384375000000003</c:v>
+                  <c:v>0.634329081632653</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>0.59021093749999998</c:v>
+                  <c:v>0.74019961734693873</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>0.68600000000000005</c:v>
+                  <c:v>0.85563265306122438</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>0.79121093750000004</c:v>
+                  <c:v>0.98062818877551006</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>0.90584375000000006</c:v>
+                  <c:v>1.1151862244897959</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>1.0298984375</c:v>
+                  <c:v>1.2593067602040815</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>1.1633749999999998</c:v>
+                  <c:v>1.4129897959183673</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>1.3062734375</c:v>
+                  <c:v>1.5762353316326529</c:v>
                 </c:pt>
                 <c:pt idx="30">
-                  <c:v>1.4585937499999999</c:v>
+                  <c:v>1.7490433673469388</c:v>
                 </c:pt>
                 <c:pt idx="31">
-                  <c:v>1.6203359374999999</c:v>
+                  <c:v>1.9314139030612243</c:v>
                 </c:pt>
                 <c:pt idx="32">
-                  <c:v>1.7914999999999999</c:v>
+                  <c:v>2.12334693877551</c:v>
                 </c:pt>
                 <c:pt idx="33">
-                  <c:v>1.9720859374999999</c:v>
+                  <c:v>2.3248424744897958</c:v>
                 </c:pt>
                 <c:pt idx="34">
-                  <c:v>2.1620937499999999</c:v>
+                  <c:v>2.5359005102040815</c:v>
                 </c:pt>
                 <c:pt idx="35">
-                  <c:v>2.3615234374999998</c:v>
+                  <c:v>2.7565210459183671</c:v>
                 </c:pt>
                 <c:pt idx="36">
-                  <c:v>2.5703749999999999</c:v>
+                  <c:v>2.9867040816326527</c:v>
                 </c:pt>
                 <c:pt idx="37">
-                  <c:v>2.7886484375</c:v>
+                  <c:v>3.2264496173469386</c:v>
                 </c:pt>
                 <c:pt idx="38">
-                  <c:v>3.0163437499999999</c:v>
+                  <c:v>3.4757576530612244</c:v>
                 </c:pt>
                 <c:pt idx="39">
-                  <c:v>3.2534609374999999</c:v>
+                  <c:v>3.7346281887755097</c:v>
                 </c:pt>
                 <c:pt idx="40">
-                  <c:v>3.5</c:v>
+                  <c:v>4.0030612244897954</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -729,11 +729,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="53064832"/>
-        <c:axId val="36420992"/>
+        <c:axId val="199956352"/>
+        <c:axId val="199957888"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="53064832"/>
+        <c:axId val="199956352"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -743,12 +743,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="36420992"/>
+        <c:crossAx val="199957888"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="36420992"/>
+        <c:axId val="199957888"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -759,7 +759,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="53064832"/>
+        <c:crossAx val="199956352"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1103,10 +1103,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A4:O45"/>
+  <dimension ref="A4:Q45"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N8" sqref="N8"/>
+    <sheetView tabSelected="1" topLeftCell="H1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="O4" sqref="O4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1147,7 +1147,7 @@
         <v>12</v>
       </c>
       <c r="N4">
-        <v>-30</v>
+        <v>-20</v>
       </c>
       <c r="O4" t="s">
         <v>13</v>
@@ -1178,7 +1178,7 @@
       </c>
       <c r="I5">
         <f>N4</f>
-        <v>-30</v>
+        <v>-20</v>
       </c>
       <c r="J5">
         <f>IF(I5&gt;N$6,L5,K5)</f>
@@ -1190,10 +1190,10 @@
       </c>
       <c r="L5" s="2">
         <f>(N$8-N$5)/((180-N$6)^2)*((I5-N$6)^2)+N$5</f>
-        <v>0.98750000000000004</v>
+        <v>0.72448979591836726</v>
       </c>
       <c r="N5">
-        <v>0.15</v>
+        <v>0.1</v>
       </c>
       <c r="O5" t="s">
         <v>14</v>
@@ -1201,19 +1201,19 @@
     </row>
     <row r="6" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A6">
-        <f>A5+$F$7</f>
+        <f t="shared" ref="A6:A45" si="0">A5+$F$7</f>
         <v>-15</v>
       </c>
       <c r="B6">
-        <f t="shared" ref="B6:B45" si="0">IF(A6&gt;F$6,D6,C6)</f>
+        <f t="shared" ref="B6:B45" si="1">IF(A6&gt;F$6,D6,C6)</f>
         <v>0</v>
       </c>
       <c r="C6" s="2">
-        <f t="shared" ref="C6:C45" si="1">F$5/(F$6-F$4)*(A6-F$4)</f>
+        <f t="shared" ref="C6:C45" si="2">F$5/(F$6-F$4)*(A6-F$4)</f>
         <v>0</v>
       </c>
       <c r="D6" s="2">
-        <f t="shared" ref="D6:D45" si="2">(F$8-F$5)/((180-F$6)^2)*((A6-F$6)^2)+F$5</f>
+        <f>(F$8-F$5)/((180-F$6)^2)*((A6-F$6)^2)+F$5</f>
         <v>0.5401785714285714</v>
       </c>
       <c r="F6">
@@ -1224,19 +1224,19 @@
       </c>
       <c r="I6">
         <f>I5+N$7</f>
-        <v>-24.75</v>
+        <v>-14.75</v>
       </c>
       <c r="J6">
         <f t="shared" ref="J6:J45" si="3">IF(I6&gt;N$6,L6,K6)</f>
-        <v>1.1250000000000001E-2</v>
+        <v>8.7500000000000008E-3</v>
       </c>
       <c r="K6" s="2">
         <f t="shared" ref="K6:K45" si="4">N$5/(N$6-N$4)*(I6-N$4)</f>
-        <v>1.1250000000000001E-2</v>
+        <v>8.7500000000000008E-3</v>
       </c>
       <c r="L6" s="2">
         <f t="shared" ref="L6:L45" si="5">(N$8-N$5)/((180-N$6)^2)*((I6-N$6)^2)+N$5</f>
-        <v>0.86658593750000001</v>
+        <v>0.61998533163265301</v>
       </c>
       <c r="N6">
         <v>40</v>
@@ -1247,19 +1247,19 @@
     </row>
     <row r="7" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A7">
-        <f>A6+$F$7</f>
+        <f t="shared" si="0"/>
         <v>-10</v>
       </c>
       <c r="B7">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="C7" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="D7" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" ref="D6:D45" si="6">(F$8-F$5)/((180-F$6)^2)*((A7-F$6)^2)+F$5</f>
         <v>0.44642857142857145</v>
       </c>
       <c r="F7">
@@ -1269,20 +1269,20 @@
         <v>16</v>
       </c>
       <c r="I7">
-        <f t="shared" ref="I7:I45" si="6">I6+N$7</f>
-        <v>-19.5</v>
+        <f t="shared" ref="I7:I45" si="7">I6+N$7</f>
+        <v>-9.5</v>
       </c>
       <c r="J7">
         <f t="shared" si="3"/>
-        <v>2.2500000000000003E-2</v>
+        <v>1.7500000000000002E-2</v>
       </c>
       <c r="K7" s="2">
-        <f t="shared" si="4"/>
-        <v>2.2500000000000003E-2</v>
+        <f>N$5/(N$6-N$4)*(I7-N$4)</f>
+        <v>1.7500000000000002E-2</v>
       </c>
       <c r="L7" s="2">
         <f t="shared" si="5"/>
-        <v>0.75509375000000001</v>
+        <v>0.52504336734693868</v>
       </c>
       <c r="N7">
         <v>5.25</v>
@@ -1293,19 +1293,19 @@
     </row>
     <row r="8" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A8">
-        <f>A7+$F$7</f>
+        <f t="shared" si="0"/>
         <v>-5</v>
       </c>
       <c r="B8">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="C8" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="D8" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v>0.36160714285714285</v>
       </c>
       <c r="F8">
@@ -1315,20 +1315,20 @@
         <v>17</v>
       </c>
       <c r="I8">
-        <f t="shared" si="6"/>
-        <v>-14.25</v>
+        <f t="shared" si="7"/>
+        <v>-4.25</v>
       </c>
       <c r="J8">
         <f t="shared" si="3"/>
-        <v>3.3750000000000002E-2</v>
+        <v>2.6250000000000002E-2</v>
       </c>
       <c r="K8" s="2">
         <f t="shared" si="4"/>
-        <v>3.3750000000000002E-2</v>
+        <v>2.6250000000000002E-2</v>
       </c>
       <c r="L8" s="2">
         <f t="shared" si="5"/>
-        <v>0.65302343750000003</v>
+        <v>0.43966390306122449</v>
       </c>
       <c r="N8">
         <v>3.5</v>
@@ -1339,1260 +1339,1271 @@
     </row>
     <row r="9" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A9">
-        <f>A8+$F$7</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="B9">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="C9" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="D9" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v>0.2857142857142857</v>
       </c>
       <c r="I9">
-        <f t="shared" si="6"/>
-        <v>-9</v>
+        <f t="shared" si="7"/>
+        <v>1</v>
       </c>
       <c r="J9">
         <f t="shared" si="3"/>
-        <v>4.5000000000000005E-2</v>
+        <v>3.5000000000000003E-2</v>
       </c>
       <c r="K9" s="2">
         <f t="shared" si="4"/>
-        <v>4.5000000000000005E-2</v>
+        <v>3.5000000000000003E-2</v>
       </c>
       <c r="L9" s="2">
         <f>(N$8-N$5)/((180-N$6)^2)*((I9-N$6)^2)+N$5</f>
-        <v>0.56037499999999996</v>
+        <v>0.36384693877551022</v>
       </c>
     </row>
     <row r="10" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A10">
-        <f>A9+$F$7</f>
+        <f t="shared" si="0"/>
         <v>5</v>
       </c>
       <c r="B10">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="C10" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="D10" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v>0.21875</v>
       </c>
       <c r="I10">
-        <f t="shared" si="6"/>
-        <v>-3.75</v>
+        <f t="shared" si="7"/>
+        <v>6.25</v>
       </c>
       <c r="J10">
         <f t="shared" si="3"/>
-        <v>5.6250000000000001E-2</v>
+        <v>4.3750000000000004E-2</v>
       </c>
       <c r="K10" s="2">
         <f t="shared" si="4"/>
-        <v>5.6250000000000001E-2</v>
+        <v>4.3750000000000004E-2</v>
       </c>
       <c r="L10" s="2">
         <f t="shared" si="5"/>
-        <v>0.47714843750000002</v>
+        <v>0.29759247448979587</v>
       </c>
     </row>
     <row r="11" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A11">
-        <f>A10+$F$7</f>
+        <f t="shared" si="0"/>
         <v>10</v>
       </c>
       <c r="B11">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="C11" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="D11" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v>0.16071428571428573</v>
       </c>
       <c r="I11">
-        <f t="shared" si="6"/>
-        <v>1.5</v>
+        <f t="shared" si="7"/>
+        <v>11.5</v>
       </c>
       <c r="J11">
-        <f t="shared" si="3"/>
-        <v>6.7500000000000004E-2</v>
+        <f>IF(I11&gt;N$6,L11,K11)</f>
+        <v>5.2500000000000005E-2</v>
       </c>
       <c r="K11" s="2">
         <f t="shared" si="4"/>
-        <v>6.7500000000000004E-2</v>
+        <v>5.2500000000000005E-2</v>
       </c>
       <c r="L11" s="2">
         <f t="shared" si="5"/>
-        <v>0.40334375</v>
+        <v>0.24090051020408162</v>
       </c>
     </row>
     <row r="12" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A12">
-        <f>A11+$F$7</f>
+        <f t="shared" si="0"/>
         <v>15</v>
       </c>
       <c r="B12">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="C12" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="D12" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v>0.11160714285714286</v>
       </c>
       <c r="I12">
-        <f t="shared" si="6"/>
-        <v>6.75</v>
+        <f t="shared" si="7"/>
+        <v>16.75</v>
       </c>
       <c r="J12">
         <f t="shared" si="3"/>
-        <v>7.8750000000000001E-2</v>
+        <v>6.1250000000000006E-2</v>
       </c>
       <c r="K12" s="2">
         <f t="shared" si="4"/>
-        <v>7.8750000000000001E-2</v>
+        <v>6.1250000000000006E-2</v>
       </c>
       <c r="L12" s="2">
-        <f t="shared" si="5"/>
-        <v>0.3389609375</v>
+        <f>(N$8-N$5)/((180-N$6)^2)*((I12-N$6)^2)+N$5</f>
+        <v>0.19377104591836736</v>
       </c>
     </row>
     <row r="13" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A13">
-        <f>A12+$F$7</f>
+        <f t="shared" si="0"/>
         <v>20</v>
       </c>
       <c r="B13">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="C13" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="D13" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v>7.1428571428571425E-2</v>
       </c>
       <c r="I13">
-        <f t="shared" si="6"/>
-        <v>12</v>
+        <f t="shared" si="7"/>
+        <v>22</v>
       </c>
       <c r="J13">
         <f t="shared" si="3"/>
-        <v>9.0000000000000011E-2</v>
+        <v>7.0000000000000007E-2</v>
       </c>
       <c r="K13" s="2">
         <f t="shared" si="4"/>
-        <v>9.0000000000000011E-2</v>
+        <v>7.0000000000000007E-2</v>
       </c>
       <c r="L13" s="2">
         <f t="shared" si="5"/>
-        <v>0.28400000000000003</v>
+        <v>0.15620408163265306</v>
       </c>
     </row>
     <row r="14" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A14">
-        <f>A13+$F$7</f>
+        <f t="shared" si="0"/>
         <v>25</v>
       </c>
       <c r="B14">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="C14" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="D14" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v>4.0178571428571432E-2</v>
       </c>
       <c r="I14">
-        <f t="shared" si="6"/>
-        <v>17.25</v>
+        <f t="shared" si="7"/>
+        <v>27.25</v>
       </c>
       <c r="J14">
         <f t="shared" si="3"/>
-        <v>0.10125000000000001</v>
+        <v>7.8750000000000001E-2</v>
       </c>
       <c r="K14" s="2">
         <f t="shared" si="4"/>
-        <v>0.10125000000000001</v>
+        <v>7.8750000000000001E-2</v>
       </c>
       <c r="L14" s="2">
         <f t="shared" si="5"/>
-        <v>0.2384609375</v>
+        <v>0.12819961734693877</v>
       </c>
     </row>
     <row r="15" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A15">
-        <f>A14+$F$7</f>
+        <f t="shared" si="0"/>
         <v>30</v>
       </c>
       <c r="B15">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="C15" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="D15" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v>1.7857142857142856E-2</v>
       </c>
       <c r="I15">
-        <f t="shared" si="6"/>
-        <v>22.5</v>
+        <f t="shared" si="7"/>
+        <v>32.5</v>
       </c>
       <c r="J15">
         <f t="shared" si="3"/>
-        <v>0.1125</v>
+        <v>8.7500000000000008E-2</v>
       </c>
       <c r="K15" s="2">
         <f t="shared" si="4"/>
-        <v>0.1125</v>
+        <v>8.7500000000000008E-2</v>
       </c>
       <c r="L15" s="2">
         <f t="shared" si="5"/>
-        <v>0.20234374999999999</v>
+        <v>0.10975765306122449</v>
       </c>
     </row>
     <row r="16" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A16">
-        <f>A15+$F$7</f>
+        <f t="shared" si="0"/>
         <v>35</v>
       </c>
       <c r="B16">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="C16" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="D16" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v>4.464285714285714E-3</v>
       </c>
       <c r="I16">
-        <f t="shared" si="6"/>
-        <v>27.75</v>
+        <f t="shared" si="7"/>
+        <v>37.75</v>
       </c>
       <c r="J16">
         <f t="shared" si="3"/>
-        <v>0.12375000000000001</v>
+        <v>9.6250000000000002E-2</v>
       </c>
       <c r="K16" s="2">
         <f t="shared" si="4"/>
-        <v>0.12375000000000001</v>
+        <v>9.6250000000000002E-2</v>
       </c>
       <c r="L16" s="2">
         <f t="shared" si="5"/>
-        <v>0.1756484375</v>
+        <v>0.10087818877551021</v>
       </c>
     </row>
     <row r="17" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A17">
-        <f>A16+$F$7</f>
+        <f t="shared" si="0"/>
         <v>40</v>
       </c>
       <c r="B17">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="C17" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="D17" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="I17">
-        <f t="shared" si="6"/>
-        <v>33</v>
+        <f t="shared" si="7"/>
+        <v>43</v>
       </c>
       <c r="J17">
         <f t="shared" si="3"/>
-        <v>0.13500000000000001</v>
+        <v>0.10156122448979592</v>
       </c>
       <c r="K17" s="2">
         <f t="shared" si="4"/>
-        <v>0.13500000000000001</v>
+        <v>0.10500000000000001</v>
       </c>
       <c r="L17" s="2">
         <f t="shared" si="5"/>
-        <v>0.15837499999999999</v>
+        <v>0.10156122448979592</v>
       </c>
     </row>
     <row r="18" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A18">
-        <f>A17+$F$7</f>
+        <f t="shared" si="0"/>
         <v>45</v>
       </c>
       <c r="B18">
-        <f t="shared" si="0"/>
+        <f>IF(A18&gt;F$6,D18,C18)</f>
         <v>4.464285714285714E-3</v>
       </c>
       <c r="C18" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="D18" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v>4.464285714285714E-3</v>
       </c>
       <c r="I18">
-        <f t="shared" si="6"/>
-        <v>38.25</v>
+        <f t="shared" si="7"/>
+        <v>48.25</v>
       </c>
       <c r="J18">
         <f t="shared" si="3"/>
-        <v>0.14625000000000002</v>
+        <v>0.11180676020408163</v>
       </c>
       <c r="K18" s="2">
         <f t="shared" si="4"/>
-        <v>0.14625000000000002</v>
+        <v>0.11375</v>
       </c>
       <c r="L18" s="2">
         <f t="shared" si="5"/>
-        <v>0.1505234375</v>
+        <v>0.11180676020408163</v>
       </c>
     </row>
     <row r="19" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A19">
-        <f>A18+$F$7</f>
+        <f t="shared" si="0"/>
         <v>50</v>
       </c>
       <c r="B19">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>1.7857142857142856E-2</v>
       </c>
       <c r="C19" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="D19" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v>1.7857142857142856E-2</v>
       </c>
       <c r="I19">
-        <f t="shared" si="6"/>
-        <v>43.5</v>
+        <f t="shared" si="7"/>
+        <v>53.5</v>
       </c>
       <c r="J19">
         <f t="shared" si="3"/>
-        <v>0.15209375</v>
+        <v>0.13161479591836733</v>
       </c>
       <c r="K19" s="2">
         <f t="shared" si="4"/>
-        <v>0.1575</v>
+        <v>0.12250000000000001</v>
       </c>
       <c r="L19" s="2">
         <f t="shared" si="5"/>
-        <v>0.15209375</v>
+        <v>0.13161479591836733</v>
       </c>
     </row>
     <row r="20" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A20">
-        <f>A19+$F$7</f>
+        <f t="shared" si="0"/>
         <v>55</v>
       </c>
       <c r="B20">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>4.0178571428571432E-2</v>
       </c>
       <c r="C20" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="D20" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v>4.0178571428571432E-2</v>
       </c>
       <c r="I20">
-        <f t="shared" si="6"/>
-        <v>48.75</v>
+        <f t="shared" si="7"/>
+        <v>58.75</v>
       </c>
       <c r="J20">
         <f t="shared" si="3"/>
-        <v>0.1630859375</v>
+        <v>0.16098533163265305</v>
       </c>
       <c r="K20" s="2">
         <f t="shared" si="4"/>
-        <v>0.16875000000000001</v>
+        <v>0.13125000000000001</v>
       </c>
       <c r="L20" s="2">
         <f t="shared" si="5"/>
-        <v>0.1630859375</v>
+        <v>0.16098533163265305</v>
       </c>
     </row>
     <row r="21" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A21">
-        <f>A20+$F$7</f>
+        <f t="shared" si="0"/>
         <v>60</v>
       </c>
       <c r="B21">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>7.1428571428571425E-2</v>
       </c>
       <c r="C21" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="D21" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v>7.1428571428571425E-2</v>
       </c>
       <c r="I21">
-        <f t="shared" si="6"/>
-        <v>54</v>
+        <f t="shared" si="7"/>
+        <v>64</v>
       </c>
       <c r="J21">
         <f t="shared" si="3"/>
-        <v>0.1835</v>
+        <v>0.19991836734693877</v>
       </c>
       <c r="K21" s="2">
         <f t="shared" si="4"/>
-        <v>0.18000000000000002</v>
+        <v>0.14000000000000001</v>
       </c>
       <c r="L21" s="2">
         <f t="shared" si="5"/>
-        <v>0.1835</v>
+        <v>0.19991836734693877</v>
       </c>
     </row>
     <row r="22" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A22">
-        <f>A21+$F$7</f>
+        <f t="shared" si="0"/>
         <v>65</v>
       </c>
       <c r="B22">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0.11160714285714286</v>
       </c>
       <c r="C22" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="D22" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v>0.11160714285714286</v>
       </c>
       <c r="I22">
-        <f t="shared" si="6"/>
-        <v>59.25</v>
+        <f t="shared" si="7"/>
+        <v>69.25</v>
       </c>
       <c r="J22">
         <f t="shared" si="3"/>
-        <v>0.21333593749999999</v>
+        <v>0.24841390306122449</v>
       </c>
       <c r="K22" s="2">
         <f t="shared" si="4"/>
-        <v>0.19125</v>
+        <v>0.14875000000000002</v>
       </c>
       <c r="L22" s="2">
         <f t="shared" si="5"/>
-        <v>0.21333593749999999</v>
+        <v>0.24841390306122449</v>
       </c>
     </row>
     <row r="23" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A23">
-        <f>A22+$F$7</f>
+        <f t="shared" si="0"/>
         <v>70</v>
       </c>
       <c r="B23">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0.16071428571428573</v>
       </c>
       <c r="C23" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="D23" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v>0.16071428571428573</v>
       </c>
       <c r="I23">
-        <f t="shared" si="6"/>
-        <v>64.5</v>
+        <f t="shared" si="7"/>
+        <v>74.5</v>
       </c>
       <c r="J23">
         <f t="shared" si="3"/>
-        <v>0.25259375000000001</v>
+        <v>0.30647193877551016</v>
       </c>
       <c r="K23" s="2">
         <f t="shared" si="4"/>
-        <v>0.20250000000000001</v>
+        <v>0.1575</v>
       </c>
       <c r="L23" s="2">
         <f t="shared" si="5"/>
-        <v>0.25259375000000001</v>
+        <v>0.30647193877551016</v>
       </c>
     </row>
     <row r="24" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A24">
-        <f>A23+$F$7</f>
+        <f t="shared" si="0"/>
         <v>75</v>
       </c>
       <c r="B24">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0.21875</v>
       </c>
       <c r="C24" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="D24" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v>0.21875</v>
       </c>
       <c r="I24">
-        <f t="shared" si="6"/>
-        <v>69.75</v>
+        <f t="shared" si="7"/>
+        <v>79.75</v>
       </c>
       <c r="J24">
         <f t="shared" si="3"/>
-        <v>0.30127343750000002</v>
+        <v>0.37409247448979588</v>
       </c>
       <c r="K24" s="2">
         <f t="shared" si="4"/>
-        <v>0.21375000000000002</v>
+        <v>0.16625000000000001</v>
       </c>
       <c r="L24" s="2">
         <f t="shared" si="5"/>
-        <v>0.30127343750000002</v>
+        <v>0.37409247448979588</v>
       </c>
     </row>
     <row r="25" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A25">
-        <f>A24+$F$7</f>
+        <f t="shared" si="0"/>
         <v>80</v>
       </c>
       <c r="B25">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0.2857142857142857</v>
       </c>
       <c r="C25" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="D25" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v>0.2857142857142857</v>
       </c>
       <c r="I25">
-        <f t="shared" si="6"/>
-        <v>75</v>
+        <f t="shared" si="7"/>
+        <v>85</v>
       </c>
       <c r="J25">
         <f t="shared" si="3"/>
-        <v>0.359375</v>
+        <v>0.45127551020408163</v>
       </c>
       <c r="K25" s="2">
         <f t="shared" si="4"/>
-        <v>0.22500000000000001</v>
+        <v>0.17500000000000002</v>
       </c>
       <c r="L25" s="2">
         <f t="shared" si="5"/>
-        <v>0.359375</v>
+        <v>0.45127551020408163</v>
       </c>
     </row>
     <row r="26" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A26">
-        <f>A25+$F$7</f>
+        <f t="shared" si="0"/>
         <v>85</v>
       </c>
       <c r="B26">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0.36160714285714285</v>
       </c>
       <c r="C26" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="D26" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v>0.36160714285714285</v>
       </c>
       <c r="I26">
-        <f t="shared" si="6"/>
-        <v>80.25</v>
+        <f t="shared" si="7"/>
+        <v>90.25</v>
       </c>
       <c r="J26">
         <f t="shared" si="3"/>
-        <v>0.42689843750000001</v>
+        <v>0.5380210459183673</v>
       </c>
       <c r="K26" s="2">
         <f t="shared" si="4"/>
-        <v>0.23625000000000002</v>
+        <v>0.18375000000000002</v>
       </c>
       <c r="L26" s="2">
         <f t="shared" si="5"/>
-        <v>0.42689843750000001</v>
+        <v>0.5380210459183673</v>
       </c>
     </row>
     <row r="27" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A27">
-        <f>A26+$F$7</f>
+        <f t="shared" si="0"/>
         <v>90</v>
       </c>
       <c r="B27">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0.44642857142857145</v>
       </c>
       <c r="C27" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="D27" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v>0.44642857142857145</v>
       </c>
       <c r="I27">
-        <f t="shared" si="6"/>
-        <v>85.5</v>
+        <f t="shared" si="7"/>
+        <v>95.5</v>
       </c>
       <c r="J27">
         <f t="shared" si="3"/>
-        <v>0.50384375000000003</v>
+        <v>0.634329081632653</v>
       </c>
       <c r="K27" s="2">
         <f t="shared" si="4"/>
-        <v>0.24750000000000003</v>
+        <v>0.1925</v>
       </c>
       <c r="L27" s="2">
         <f t="shared" si="5"/>
-        <v>0.50384375000000003</v>
+        <v>0.634329081632653</v>
       </c>
     </row>
     <row r="28" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A28">
-        <f>A27+$F$7</f>
+        <f t="shared" si="0"/>
         <v>95</v>
       </c>
       <c r="B28">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0.5401785714285714</v>
       </c>
       <c r="C28" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="D28" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v>0.5401785714285714</v>
       </c>
       <c r="I28">
-        <f t="shared" si="6"/>
-        <v>90.75</v>
+        <f t="shared" si="7"/>
+        <v>100.75</v>
       </c>
       <c r="J28">
         <f t="shared" si="3"/>
-        <v>0.59021093749999998</v>
+        <v>0.74019961734693873</v>
       </c>
       <c r="K28" s="2">
         <f t="shared" si="4"/>
-        <v>0.25875000000000004</v>
+        <v>0.20125000000000001</v>
       </c>
       <c r="L28" s="2">
         <f t="shared" si="5"/>
-        <v>0.59021093749999998</v>
+        <v>0.74019961734693873</v>
       </c>
     </row>
     <row r="29" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A29">
-        <f>A28+$F$7</f>
+        <f t="shared" si="0"/>
         <v>100</v>
       </c>
       <c r="B29">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0.6428571428571429</v>
       </c>
       <c r="C29" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="D29" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v>0.6428571428571429</v>
       </c>
       <c r="I29">
-        <f t="shared" si="6"/>
-        <v>96</v>
+        <f t="shared" si="7"/>
+        <v>106</v>
       </c>
       <c r="J29">
         <f t="shared" si="3"/>
-        <v>0.68600000000000005</v>
+        <v>0.85563265306122438</v>
       </c>
       <c r="K29" s="2">
         <f t="shared" si="4"/>
-        <v>0.27</v>
+        <v>0.21000000000000002</v>
       </c>
       <c r="L29" s="2">
         <f t="shared" si="5"/>
-        <v>0.68600000000000005</v>
+        <v>0.85563265306122438</v>
       </c>
     </row>
     <row r="30" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A30">
-        <f>A29+$F$7</f>
+        <f t="shared" si="0"/>
         <v>105</v>
       </c>
       <c r="B30">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0.7544642857142857</v>
       </c>
       <c r="C30" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="D30" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v>0.7544642857142857</v>
       </c>
       <c r="I30">
-        <f t="shared" si="6"/>
-        <v>101.25</v>
+        <f t="shared" si="7"/>
+        <v>111.25</v>
       </c>
       <c r="J30">
         <f t="shared" si="3"/>
-        <v>0.79121093750000004</v>
+        <v>0.98062818877551006</v>
       </c>
       <c r="K30" s="2">
         <f t="shared" si="4"/>
-        <v>0.28125</v>
+        <v>0.21875000000000003</v>
       </c>
       <c r="L30" s="2">
         <f t="shared" si="5"/>
-        <v>0.79121093750000004</v>
+        <v>0.98062818877551006</v>
       </c>
     </row>
     <row r="31" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A31">
-        <f>A30+$F$7</f>
+        <f t="shared" si="0"/>
         <v>110</v>
       </c>
       <c r="B31">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0.875</v>
       </c>
       <c r="C31" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="D31" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v>0.875</v>
       </c>
       <c r="I31">
-        <f t="shared" si="6"/>
-        <v>106.5</v>
+        <f t="shared" si="7"/>
+        <v>116.5</v>
       </c>
       <c r="J31">
         <f t="shared" si="3"/>
-        <v>0.90584375000000006</v>
+        <v>1.1151862244897959</v>
       </c>
       <c r="K31" s="2">
         <f t="shared" si="4"/>
-        <v>0.29250000000000004</v>
+        <v>0.22750000000000001</v>
       </c>
       <c r="L31" s="2">
         <f t="shared" si="5"/>
-        <v>0.90584375000000006</v>
+        <v>1.1151862244897959</v>
       </c>
     </row>
     <row r="32" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A32">
-        <f>A31+$F$7</f>
+        <f t="shared" si="0"/>
         <v>115</v>
       </c>
       <c r="B32">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>1.0044642857142858</v>
       </c>
       <c r="C32" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="D32" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v>1.0044642857142858</v>
       </c>
       <c r="I32">
-        <f t="shared" si="6"/>
-        <v>111.75</v>
+        <f t="shared" si="7"/>
+        <v>121.75</v>
       </c>
       <c r="J32">
         <f t="shared" si="3"/>
-        <v>1.0298984375</v>
+        <v>1.2593067602040815</v>
       </c>
       <c r="K32" s="2">
         <f t="shared" si="4"/>
-        <v>0.30375000000000002</v>
+        <v>0.23625000000000002</v>
       </c>
       <c r="L32" s="2">
         <f t="shared" si="5"/>
-        <v>1.0298984375</v>
-      </c>
-    </row>
-    <row r="33" spans="1:12" x14ac:dyDescent="0.25">
+        <v>1.2593067602040815</v>
+      </c>
+    </row>
+    <row r="33" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A33">
-        <f>A32+$F$7</f>
+        <f t="shared" si="0"/>
         <v>120</v>
       </c>
       <c r="B33">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>1.1428571428571428</v>
       </c>
       <c r="C33" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="D33" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v>1.1428571428571428</v>
       </c>
       <c r="I33">
-        <f t="shared" si="6"/>
-        <v>117</v>
+        <f t="shared" si="7"/>
+        <v>127</v>
       </c>
       <c r="J33">
         <f t="shared" si="3"/>
-        <v>1.1633749999999998</v>
+        <v>1.4129897959183673</v>
       </c>
       <c r="K33" s="2">
         <f t="shared" si="4"/>
+        <v>0.24500000000000002</v>
+      </c>
+      <c r="L33" s="2">
+        <f t="shared" si="5"/>
+        <v>1.4129897959183673</v>
+      </c>
+    </row>
+    <row r="34" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A34">
+        <f t="shared" si="0"/>
+        <v>125</v>
+      </c>
+      <c r="B34">
+        <f t="shared" si="1"/>
+        <v>1.2901785714285714</v>
+      </c>
+      <c r="C34" s="2">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="D34" s="2">
+        <f t="shared" si="6"/>
+        <v>1.2901785714285714</v>
+      </c>
+      <c r="I34">
+        <f t="shared" si="7"/>
+        <v>132.25</v>
+      </c>
+      <c r="J34">
+        <f t="shared" si="3"/>
+        <v>1.5762353316326529</v>
+      </c>
+      <c r="K34" s="2">
+        <f t="shared" si="4"/>
+        <v>0.25375000000000003</v>
+      </c>
+      <c r="L34" s="2">
+        <f t="shared" si="5"/>
+        <v>1.5762353316326529</v>
+      </c>
+      <c r="Q34">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="35" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A35">
+        <f t="shared" si="0"/>
+        <v>130</v>
+      </c>
+      <c r="B35">
+        <f t="shared" si="1"/>
+        <v>1.4464285714285714</v>
+      </c>
+      <c r="C35" s="2">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="D35" s="2">
+        <f t="shared" si="6"/>
+        <v>1.4464285714285714</v>
+      </c>
+      <c r="I35">
+        <f t="shared" si="7"/>
+        <v>137.5</v>
+      </c>
+      <c r="J35">
+        <f t="shared" si="3"/>
+        <v>1.7490433673469388</v>
+      </c>
+      <c r="K35" s="2">
+        <f t="shared" si="4"/>
+        <v>0.26250000000000001</v>
+      </c>
+      <c r="L35" s="2">
+        <f t="shared" si="5"/>
+        <v>1.7490433673469388</v>
+      </c>
+      <c r="Q35">
+        <f>Q34/2</f>
+        <v>140</v>
+      </c>
+    </row>
+    <row r="36" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A36">
+        <f t="shared" si="0"/>
+        <v>135</v>
+      </c>
+      <c r="B36">
+        <f t="shared" si="1"/>
+        <v>1.6116071428571428</v>
+      </c>
+      <c r="C36" s="2">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="D36" s="2">
+        <f t="shared" si="6"/>
+        <v>1.6116071428571428</v>
+      </c>
+      <c r="I36">
+        <f t="shared" si="7"/>
+        <v>142.75</v>
+      </c>
+      <c r="J36">
+        <f t="shared" si="3"/>
+        <v>1.9314139030612243</v>
+      </c>
+      <c r="K36" s="2">
+        <f t="shared" si="4"/>
+        <v>0.27124999999999999</v>
+      </c>
+      <c r="L36" s="2">
+        <f t="shared" si="5"/>
+        <v>1.9314139030612243</v>
+      </c>
+      <c r="Q36">
+        <f>SQRT(Q35)/2</f>
+        <v>5.9160797830996161</v>
+      </c>
+    </row>
+    <row r="37" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A37">
+        <f t="shared" si="0"/>
+        <v>140</v>
+      </c>
+      <c r="B37">
+        <f t="shared" si="1"/>
+        <v>1.7857142857142858</v>
+      </c>
+      <c r="C37" s="2">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="D37" s="2">
+        <f t="shared" si="6"/>
+        <v>1.7857142857142858</v>
+      </c>
+      <c r="I37">
+        <f t="shared" si="7"/>
+        <v>148</v>
+      </c>
+      <c r="J37">
+        <f t="shared" si="3"/>
+        <v>2.12334693877551</v>
+      </c>
+      <c r="K37" s="2">
+        <f t="shared" si="4"/>
+        <v>0.28000000000000003</v>
+      </c>
+      <c r="L37" s="2">
+        <f t="shared" si="5"/>
+        <v>2.12334693877551</v>
+      </c>
+    </row>
+    <row r="38" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A38">
+        <f t="shared" si="0"/>
+        <v>145</v>
+      </c>
+      <c r="B38">
+        <f t="shared" si="1"/>
+        <v>1.96875</v>
+      </c>
+      <c r="C38" s="2">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="D38" s="2">
+        <f t="shared" si="6"/>
+        <v>1.96875</v>
+      </c>
+      <c r="I38">
+        <f t="shared" si="7"/>
+        <v>153.25</v>
+      </c>
+      <c r="J38">
+        <f t="shared" si="3"/>
+        <v>2.3248424744897958</v>
+      </c>
+      <c r="K38" s="2">
+        <f t="shared" si="4"/>
+        <v>0.28875000000000001</v>
+      </c>
+      <c r="L38" s="2">
+        <f t="shared" si="5"/>
+        <v>2.3248424744897958</v>
+      </c>
+    </row>
+    <row r="39" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A39">
+        <f t="shared" si="0"/>
+        <v>150</v>
+      </c>
+      <c r="B39">
+        <f t="shared" si="1"/>
+        <v>2.1607142857142856</v>
+      </c>
+      <c r="C39" s="2">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="D39" s="2">
+        <f t="shared" si="6"/>
+        <v>2.1607142857142856</v>
+      </c>
+      <c r="I39">
+        <f t="shared" si="7"/>
+        <v>158.5</v>
+      </c>
+      <c r="J39">
+        <f t="shared" si="3"/>
+        <v>2.5359005102040815</v>
+      </c>
+      <c r="K39" s="2">
+        <f t="shared" si="4"/>
+        <v>0.29750000000000004</v>
+      </c>
+      <c r="L39" s="2">
+        <f t="shared" si="5"/>
+        <v>2.5359005102040815</v>
+      </c>
+    </row>
+    <row r="40" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A40">
+        <f t="shared" si="0"/>
+        <v>155</v>
+      </c>
+      <c r="B40">
+        <f t="shared" si="1"/>
+        <v>2.3616071428571428</v>
+      </c>
+      <c r="C40" s="2">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="D40" s="2">
+        <f t="shared" si="6"/>
+        <v>2.3616071428571428</v>
+      </c>
+      <c r="I40">
+        <f t="shared" si="7"/>
+        <v>163.75</v>
+      </c>
+      <c r="J40">
+        <f t="shared" si="3"/>
+        <v>2.7565210459183671</v>
+      </c>
+      <c r="K40" s="2">
+        <f t="shared" si="4"/>
+        <v>0.30625000000000002</v>
+      </c>
+      <c r="L40" s="2">
+        <f t="shared" si="5"/>
+        <v>2.7565210459183671</v>
+      </c>
+    </row>
+    <row r="41" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A41">
+        <f t="shared" si="0"/>
+        <v>160</v>
+      </c>
+      <c r="B41">
+        <f t="shared" si="1"/>
+        <v>2.5714285714285716</v>
+      </c>
+      <c r="C41" s="2">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="D41" s="2">
+        <f t="shared" si="6"/>
+        <v>2.5714285714285716</v>
+      </c>
+      <c r="I41">
+        <f t="shared" si="7"/>
+        <v>169</v>
+      </c>
+      <c r="J41">
+        <f t="shared" si="3"/>
+        <v>2.9867040816326527</v>
+      </c>
+      <c r="K41" s="2">
+        <f t="shared" si="4"/>
         <v>0.315</v>
       </c>
-      <c r="L33" s="2">
-        <f t="shared" si="5"/>
-        <v>1.1633749999999998</v>
-      </c>
-    </row>
-    <row r="34" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A34">
-        <f>A33+$F$7</f>
-        <v>125</v>
-      </c>
-      <c r="B34">
-        <f t="shared" si="0"/>
-        <v>1.2901785714285714</v>
-      </c>
-      <c r="C34" s="2">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="D34" s="2">
-        <f t="shared" si="2"/>
-        <v>1.2901785714285714</v>
-      </c>
-      <c r="I34">
-        <f t="shared" si="6"/>
-        <v>122.25</v>
-      </c>
-      <c r="J34">
-        <f t="shared" si="3"/>
-        <v>1.3062734375</v>
-      </c>
-      <c r="K34" s="2">
-        <f t="shared" si="4"/>
-        <v>0.32625000000000004</v>
-      </c>
-      <c r="L34" s="2">
-        <f t="shared" si="5"/>
-        <v>1.3062734375</v>
-      </c>
-    </row>
-    <row r="35" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A35">
-        <f>A34+$F$7</f>
-        <v>130</v>
-      </c>
-      <c r="B35">
-        <f t="shared" si="0"/>
-        <v>1.4464285714285714</v>
-      </c>
-      <c r="C35" s="2">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="D35" s="2">
-        <f t="shared" si="2"/>
-        <v>1.4464285714285714</v>
-      </c>
-      <c r="I35">
-        <f t="shared" si="6"/>
-        <v>127.5</v>
-      </c>
-      <c r="J35">
-        <f t="shared" si="3"/>
-        <v>1.4585937499999999</v>
-      </c>
-      <c r="K35" s="2">
-        <f t="shared" si="4"/>
-        <v>0.33750000000000002</v>
-      </c>
-      <c r="L35" s="2">
-        <f t="shared" si="5"/>
-        <v>1.4585937499999999</v>
-      </c>
-    </row>
-    <row r="36" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A36">
-        <f>A35+$F$7</f>
-        <v>135</v>
-      </c>
-      <c r="B36">
-        <f t="shared" si="0"/>
-        <v>1.6116071428571428</v>
-      </c>
-      <c r="C36" s="2">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="D36" s="2">
-        <f t="shared" si="2"/>
-        <v>1.6116071428571428</v>
-      </c>
-      <c r="I36">
-        <f t="shared" si="6"/>
-        <v>132.75</v>
-      </c>
-      <c r="J36">
-        <f t="shared" si="3"/>
-        <v>1.6203359374999999</v>
-      </c>
-      <c r="K36" s="2">
-        <f t="shared" si="4"/>
-        <v>0.34875</v>
-      </c>
-      <c r="L36" s="2">
-        <f t="shared" si="5"/>
-        <v>1.6203359374999999</v>
-      </c>
-    </row>
-    <row r="37" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A37">
-        <f>A36+$F$7</f>
-        <v>140</v>
-      </c>
-      <c r="B37">
-        <f t="shared" si="0"/>
-        <v>1.7857142857142858</v>
-      </c>
-      <c r="C37" s="2">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="D37" s="2">
-        <f t="shared" si="2"/>
-        <v>1.7857142857142858</v>
-      </c>
-      <c r="I37">
-        <f t="shared" si="6"/>
-        <v>138</v>
-      </c>
-      <c r="J37">
-        <f t="shared" si="3"/>
-        <v>1.7914999999999999</v>
-      </c>
-      <c r="K37" s="2">
-        <f t="shared" si="4"/>
-        <v>0.36000000000000004</v>
-      </c>
-      <c r="L37" s="2">
-        <f t="shared" si="5"/>
-        <v>1.7914999999999999</v>
-      </c>
-    </row>
-    <row r="38" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A38">
-        <f>A37+$F$7</f>
-        <v>145</v>
-      </c>
-      <c r="B38">
-        <f t="shared" si="0"/>
-        <v>1.96875</v>
-      </c>
-      <c r="C38" s="2">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="D38" s="2">
-        <f t="shared" si="2"/>
-        <v>1.96875</v>
-      </c>
-      <c r="I38">
-        <f t="shared" si="6"/>
-        <v>143.25</v>
-      </c>
-      <c r="J38">
-        <f t="shared" si="3"/>
-        <v>1.9720859374999999</v>
-      </c>
-      <c r="K38" s="2">
-        <f t="shared" si="4"/>
-        <v>0.37125000000000002</v>
-      </c>
-      <c r="L38" s="2">
-        <f t="shared" si="5"/>
-        <v>1.9720859374999999</v>
-      </c>
-    </row>
-    <row r="39" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A39">
-        <f>A38+$F$7</f>
-        <v>150</v>
-      </c>
-      <c r="B39">
-        <f t="shared" si="0"/>
-        <v>2.1607142857142856</v>
-      </c>
-      <c r="C39" s="2">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="D39" s="2">
-        <f t="shared" si="2"/>
-        <v>2.1607142857142856</v>
-      </c>
-      <c r="I39">
-        <f t="shared" si="6"/>
-        <v>148.5</v>
-      </c>
-      <c r="J39">
-        <f t="shared" si="3"/>
-        <v>2.1620937499999999</v>
-      </c>
-      <c r="K39" s="2">
-        <f t="shared" si="4"/>
-        <v>0.38250000000000001</v>
-      </c>
-      <c r="L39" s="2">
-        <f t="shared" si="5"/>
-        <v>2.1620937499999999</v>
-      </c>
-    </row>
-    <row r="40" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A40">
-        <f>A39+$F$7</f>
-        <v>155</v>
-      </c>
-      <c r="B40">
-        <f t="shared" si="0"/>
-        <v>2.3616071428571428</v>
-      </c>
-      <c r="C40" s="2">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="D40" s="2">
-        <f t="shared" si="2"/>
-        <v>2.3616071428571428</v>
-      </c>
-      <c r="I40">
-        <f t="shared" si="6"/>
-        <v>153.75</v>
-      </c>
-      <c r="J40">
-        <f t="shared" si="3"/>
-        <v>2.3615234374999998</v>
-      </c>
-      <c r="K40" s="2">
-        <f t="shared" si="4"/>
-        <v>0.39375000000000004</v>
-      </c>
-      <c r="L40" s="2">
-        <f t="shared" si="5"/>
-        <v>2.3615234374999998</v>
-      </c>
-    </row>
-    <row r="41" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A41">
-        <f>A40+$F$7</f>
-        <v>160</v>
-      </c>
-      <c r="B41">
-        <f t="shared" si="0"/>
-        <v>2.5714285714285716</v>
-      </c>
-      <c r="C41" s="2">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="D41" s="2">
-        <f t="shared" si="2"/>
-        <v>2.5714285714285716</v>
-      </c>
-      <c r="I41">
-        <f t="shared" si="6"/>
-        <v>159</v>
-      </c>
-      <c r="J41">
-        <f t="shared" si="3"/>
-        <v>2.5703749999999999</v>
-      </c>
-      <c r="K41" s="2">
-        <f t="shared" si="4"/>
-        <v>0.40500000000000003</v>
-      </c>
       <c r="L41" s="2">
         <f t="shared" si="5"/>
-        <v>2.5703749999999999</v>
-      </c>
-    </row>
-    <row r="42" spans="1:12" x14ac:dyDescent="0.25">
+        <v>2.9867040816326527</v>
+      </c>
+    </row>
+    <row r="42" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A42">
-        <f>A41+$F$7</f>
+        <f t="shared" si="0"/>
         <v>165</v>
       </c>
       <c r="B42">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>2.7901785714285716</v>
       </c>
       <c r="C42" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="D42" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v>2.7901785714285716</v>
       </c>
       <c r="I42">
-        <f t="shared" si="6"/>
-        <v>164.25</v>
+        <f t="shared" si="7"/>
+        <v>174.25</v>
       </c>
       <c r="J42">
         <f t="shared" si="3"/>
-        <v>2.7886484375</v>
+        <v>3.2264496173469386</v>
       </c>
       <c r="K42" s="2">
         <f t="shared" si="4"/>
-        <v>0.41625000000000001</v>
+        <v>0.32375000000000004</v>
       </c>
       <c r="L42" s="2">
         <f t="shared" si="5"/>
-        <v>2.7886484375</v>
-      </c>
-    </row>
-    <row r="43" spans="1:12" x14ac:dyDescent="0.25">
+        <v>3.2264496173469386</v>
+      </c>
+    </row>
+    <row r="43" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A43">
-        <f>A42+$F$7</f>
+        <f t="shared" si="0"/>
         <v>170</v>
       </c>
       <c r="B43">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>3.0178571428571428</v>
       </c>
       <c r="C43" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="D43" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v>3.0178571428571428</v>
       </c>
       <c r="I43">
-        <f t="shared" si="6"/>
-        <v>169.5</v>
+        <f t="shared" si="7"/>
+        <v>179.5</v>
       </c>
       <c r="J43">
         <f t="shared" si="3"/>
-        <v>3.0163437499999999</v>
+        <v>3.4757576530612244</v>
       </c>
       <c r="K43" s="2">
         <f t="shared" si="4"/>
-        <v>0.42750000000000005</v>
+        <v>0.33250000000000002</v>
       </c>
       <c r="L43" s="2">
         <f t="shared" si="5"/>
-        <v>3.0163437499999999</v>
-      </c>
-    </row>
-    <row r="44" spans="1:12" x14ac:dyDescent="0.25">
+        <v>3.4757576530612244</v>
+      </c>
+    </row>
+    <row r="44" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A44">
-        <f>A43+$F$7</f>
+        <f t="shared" si="0"/>
         <v>175</v>
       </c>
       <c r="B44">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>3.2544642857142856</v>
       </c>
       <c r="C44" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="D44" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v>3.2544642857142856</v>
       </c>
       <c r="I44">
-        <f t="shared" si="6"/>
-        <v>174.75</v>
+        <f t="shared" si="7"/>
+        <v>184.75</v>
       </c>
       <c r="J44">
         <f t="shared" si="3"/>
-        <v>3.2534609374999999</v>
+        <v>3.7346281887755097</v>
       </c>
       <c r="K44" s="2">
         <f t="shared" si="4"/>
-        <v>0.43875000000000003</v>
+        <v>0.34125</v>
       </c>
       <c r="L44" s="2">
         <f t="shared" si="5"/>
-        <v>3.2534609374999999</v>
-      </c>
-    </row>
-    <row r="45" spans="1:12" x14ac:dyDescent="0.25">
+        <v>3.7346281887755097</v>
+      </c>
+    </row>
+    <row r="45" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A45">
-        <f>A44+$F$7</f>
+        <f t="shared" si="0"/>
         <v>180</v>
       </c>
       <c r="B45">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>3.5</v>
       </c>
       <c r="C45" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="D45" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v>3.5</v>
       </c>
       <c r="I45">
-        <f t="shared" si="6"/>
-        <v>180</v>
+        <f t="shared" si="7"/>
+        <v>190</v>
       </c>
       <c r="J45">
         <f t="shared" si="3"/>
-        <v>3.5</v>
+        <v>4.0030612244897954</v>
       </c>
       <c r="K45" s="2">
         <f t="shared" si="4"/>
-        <v>0.45</v>
+        <v>0.35000000000000003</v>
       </c>
       <c r="L45" s="2">
         <f t="shared" si="5"/>
-        <v>3.5</v>
+        <v>4.0030612244897954</v>
       </c>
     </row>
   </sheetData>

</xml_diff>